<commit_message>
first example is done
</commit_message>
<xml_diff>
--- a/tests/example_spreadsheet.xlsx
+++ b/tests/example_spreadsheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t xml:space="preserve">dcterms:identifier</t>
   </si>
@@ -41,7 +41,7 @@
     <t xml:space="preserve">dcterms:license</t>
   </si>
   <si>
-    <t xml:space="preserve">dcat:hasCurrentVersion</t>
+    <t xml:space="preserve">dcat:version</t>
   </si>
   <si>
     <t xml:space="preserve">dcat:theme</t>
@@ -62,6 +62,9 @@
     <t xml:space="preserve">dcat:distribution</t>
   </si>
   <si>
+    <t xml:space="preserve">dcterms:modified</t>
+  </si>
+  <si>
     <t xml:space="preserve">test data</t>
   </si>
   <si>
@@ -125,10 +128,7 @@
     <t xml:space="preserve">dcterms:format</t>
   </si>
   <si>
-    <t xml:space="preserve">dcterms:modified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.example.com/test.xslx</t>
+    <t xml:space="preserve">https://www.example.com/test.xslx</t>
   </si>
   <si>
     <t xml:space="preserve">excel</t>
@@ -137,7 +137,7 @@
     <t xml:space="preserve">0.1.0</t>
   </si>
   <si>
-    <t xml:space="preserve">www.example.org/lineagetest.avro</t>
+    <t xml:space="preserve">https://www.example.org/lineagetest.avro</t>
   </si>
   <si>
     <t xml:space="preserve">https://avro.apache.org/docs/1.12.0/</t>
@@ -154,7 +154,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -175,13 +175,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -233,7 +226,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -246,15 +239,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -381,10 +370,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -441,78 +430,84 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>12345</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>2010</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <v>45580</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>73956</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>2011</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L3" s="1" t="n">
         <f aca="false">A2</f>
@@ -520,6 +515,9 @@
       </c>
       <c r="M3" s="1" t="n">
         <v>94759</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>45582</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +544,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -562,16 +560,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -587,7 +585,7 @@
       <c r="D2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="3" t="n">
         <v>45580</v>
       </c>
     </row>
@@ -598,20 +596,20 @@
       <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="3" t="n">
         <v>45582</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="www.example.com/test.xslx"/>
-    <hyperlink ref="B3" r:id="rId2" display="www.example.org/lineagetest.avro"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.example.com/test.xslx"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www"/>
     <hyperlink ref="C3" r:id="rId3" display="https://avro.apache.org/docs/1.12.0/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
testing links in headers
</commit_message>
<xml_diff>
--- a/tests/example_spreadsheet.xlsx
+++ b/tests/example_spreadsheet.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Distributions" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Concepts" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t xml:space="preserve">dcterms:identifier</t>
   </si>
@@ -113,7 +114,7 @@
     <t xml:space="preserve">0.3.3</t>
   </si>
   <si>
-    <t xml:space="preserve">test, lineage</t>
+    <t xml:space="preserve">lineage, catalog</t>
   </si>
   <si>
     <t xml:space="preserve">France</t>
@@ -144,6 +145,42 @@
   </si>
   <si>
     <t xml:space="preserve">4.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skos:prefLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skos:definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skos:example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iu34jkAWD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">an excersize in determining if something works or behaves as expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I’m testing if this works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catalog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdfjlhgfvrkhlsfd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a curated collection of datasets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lineage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fdcshjnfdscahjn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A discription of where something comes from or how it was created</t>
   </si>
 </sst>
 </file>
@@ -372,8 +409,8 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -543,7 +580,7 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -609,7 +646,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://www.example.com/test.xslx"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://www"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.example.org/lineagetest.avro"/>
     <hyperlink ref="C3" r:id="rId3" display="https://avro.apache.org/docs/1.12.0/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -620,4 +657,83 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
alvaro better be pleased
</commit_message>
<xml_diff>
--- a/tests/example_spreadsheet.xlsx
+++ b/tests/example_spreadsheet.xlsx
@@ -11,6 +11,8 @@
     <sheet name="Datasets" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Distributions" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Concepts" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Metrics" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="QualityMeasurements" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="108">
   <si>
     <t xml:space="preserve">dcterms:identifier</t>
   </si>
@@ -123,6 +125,36 @@
     <t xml:space="preserve">test</t>
   </si>
   <si>
+    <t xml:space="preserve">ewrcqwfeb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existing wind on-shore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data set contains data on capacity factors of on-shore wind across different GIS regions as a time series since 1980 to 2022 on hourly basis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info@mopo.eu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind, offshore, capacity factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1980-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skfhafuku</t>
+  </si>
+  <si>
     <t xml:space="preserve">dcat:accessURL</t>
   </si>
   <si>
@@ -147,6 +179,15 @@
     <t xml:space="preserve">4.5.1</t>
   </si>
   <si>
+    <t xml:space="preserve">https://data.dtu.dk/ndownloader/files/34972672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-05-02</t>
+  </si>
+  <si>
     <t xml:space="preserve">skos:prefLabel</t>
   </si>
   <si>
@@ -156,6 +197,9 @@
     <t xml:space="preserve">skos:example</t>
   </si>
   <si>
+    <t xml:space="preserve">skos:altLabel</t>
+  </si>
+  <si>
     <t xml:space="preserve">iu34jkAWD</t>
   </si>
   <si>
@@ -181,17 +225,142 @@
   </si>
   <si>
     <t xml:space="preserve">A discription of where something comes from or how it was created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fajfafl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind as an energy source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">offshore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weruEF8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">installed on the sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">973I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the fraction of installed capacity that was or is available at a given moment in time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dqv:expectedDataType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dqv:inDimension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kd84jsd8wksyf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">response time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the time it takes between when a request was made and when a response was provided, measured in seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xsd:float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iso:Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja9EJDS8E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fraction of compliant records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the fraction (between 0 and 1) of the amount of records in the dataset that complies to the schema as defined by some specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iso:Compliance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mwqd83k93k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the number of unique records in the dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xsd:int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iso:Completeness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jkdsfAFdfgsdfg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all countries present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we have data representing the capacity for all countries within the EU usecase. measured as a fraction between the collumns in the dataset and the expected columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dqv:computedOn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dqv:isMeasurementOf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dqv:value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov:generatedAtTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jQ8PY1234LJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-10-19T14:46:01+0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skekxmkr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-10-19T14:46:51+0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keq3ek843</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-11-19T14:46:51+0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asFSMAWBAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-10-21T15:01:34+0000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -219,6 +388,18 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -263,7 +444,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -282,6 +463,30 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -407,16 +612,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.38"/>
@@ -557,11 +762,53 @@
         <v>45582</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="6" t="n">
+        <v>45586</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="jdoe@example.com"/>
     <hyperlink ref="E3" r:id="rId2" display="jane@example.org"/>
     <hyperlink ref="F3" r:id="rId3" display="https://opensource.org/licenses/Apache-2.0"/>
+    <hyperlink ref="E4" r:id="rId4" display="info@mopo.eu"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -578,10 +825,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -597,10 +844,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -614,13 +861,13 @@
         <v>23456</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>45580</v>
@@ -631,16 +878,33 @@
         <v>94759</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>45582</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -664,67 +928,336 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>43</v>
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>46</v>
+      <c r="B2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>49</v>
+      <c r="A3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>52</v>
+      <c r="A4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.96"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.27"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>73956</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>73956</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0.975</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>12345</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>275937582</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added supply chain analysis
</commit_message>
<xml_diff>
--- a/tests/example_spreadsheet.xlsx
+++ b/tests/example_spreadsheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="122">
   <si>
     <t xml:space="preserve">dcterms:identifier</t>
   </si>
@@ -125,6 +125,9 @@
     <t xml:space="preserve">test</t>
   </si>
   <si>
+    <t xml:space="preserve">12345, </t>
+  </si>
+  <si>
     <t xml:space="preserve">ewrcqwfeb</t>
   </si>
   <si>
@@ -158,6 +161,36 @@
     <t xml:space="preserve">skfhafuku</t>
   </si>
   <si>
+    <t xml:space="preserve">dsdfadf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tst data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">another test data set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uuidea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test@test.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cc—by 4.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind, lineage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belgium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdfasdbf</t>
+  </si>
+  <si>
     <t xml:space="preserve">dcat:accessURL</t>
   </si>
   <si>
@@ -189,6 +222,12 @@
   </si>
   <si>
     <t xml:space="preserve">2022-05-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.example.comtst.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.6.1</t>
   </si>
   <si>
     <t xml:space="preserve">skos:prefLabel</t>
@@ -362,7 +401,7 @@
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -383,6 +422,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -434,7 +480,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -456,6 +502,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -590,10 +640,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -729,9 +779,8 @@
       <c r="K3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="1" t="n">
-        <f aca="false">A2</f>
-        <v>12345</v>
+      <c r="L3" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>94759</v>
@@ -742,19 +791,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>18</v>
@@ -763,24 +812,65 @@
         <v>0.4</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N4" s="5" t="n">
+        <v>45586</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5" s="5" t="n">
         <v>45586</v>
       </c>
     </row>
@@ -790,6 +880,7 @@
     <hyperlink ref="E3" r:id="rId2" display="jane@example.org"/>
     <hyperlink ref="F3" r:id="rId3" display="https://opensource.org/licenses/Apache-2.0"/>
     <hyperlink ref="E4" r:id="rId4" display="info@mopo.eu"/>
+    <hyperlink ref="E5" r:id="rId5" display="test@test.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -806,10 +897,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="N5 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -825,10 +916,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -842,13 +933,13 @@
         <v>23456</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>45580</v>
@@ -859,13 +950,13 @@
         <v>94759</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>45582</v>
@@ -873,19 +964,36 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>54</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -893,6 +1001,7 @@
     <hyperlink ref="B2" r:id="rId1" display="https://www.example.com/test.xslx"/>
     <hyperlink ref="B3" r:id="rId2" display="https://www.example.org/lineagetest.avro"/>
     <hyperlink ref="C3" r:id="rId3" display="https://avro.apache.org/docs/1.12.0/"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www.example.comtst.csv"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -911,8 +1020,8 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="1" sqref="N5 E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -924,19 +1033,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,71 +1053,71 @@
         <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1029,8 +1138,8 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="N5 C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1046,84 +1155,84 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1144,8 +1253,8 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="1" sqref="N5 L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1161,84 +1270,84 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>100</v>
+        <v>112</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>73956</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>5.46</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>102</v>
+      <c r="E2" s="8" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>73956</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0.975</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>104</v>
+      <c r="E3" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>12345</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>275937582</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>106</v>
+      <c r="E4" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>108</v>
+      <c r="E5" s="8" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complicated supply chain analysis
</commit_message>
<xml_diff>
--- a/tests/example_spreadsheet.xlsx
+++ b/tests/example_spreadsheet.xlsx
@@ -125,7 +125,7 @@
     <t xml:space="preserve">test</t>
   </si>
   <si>
-    <t xml:space="preserve">12345, </t>
+    <t xml:space="preserve">12345, dsdfadf</t>
   </si>
   <si>
     <t xml:space="preserve">ewrcqwfeb</t>
@@ -642,8 +642,8 @@
   </sheetPr>
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -900,7 +900,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="N5 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1021,7 +1021,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="1" sqref="N5 E7"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1139,7 +1139,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="N5 C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1254,7 +1254,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="1" sqref="N5 L2"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
index is now generated from catalog data
</commit_message>
<xml_diff>
--- a/tests/example_spreadsheet.xlsx
+++ b/tests/example_spreadsheet.xlsx
@@ -8,11 +8,12 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Datasets" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Distributions" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Concepts" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Metrics" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="QualityMeasurements" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="DataCatalog" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Datasets" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Distributions" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Concepts" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Metrics" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="QualityMeasurements" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,32 +25,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="127">
+  <si>
+    <t xml:space="preserve">dcterms:title</t>
+  </si>
   <si>
     <t xml:space="preserve">dcterms:identifier</t>
   </si>
   <si>
-    <t xml:space="preserve">dcterms:title</t>
-  </si>
-  <si>
     <t xml:space="preserve">dcterms:description</t>
   </si>
   <si>
+    <t xml:space="preserve">dcterms:license</t>
+  </si>
+  <si>
     <t xml:space="preserve">dcterms:publisher</t>
   </si>
   <si>
+    <t xml:space="preserve">dcat:theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test data catalog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdsfvfakhflkauh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a data catalog to test different functions of the SimpleMDDataCatalog project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cc-by-sa 4.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SimpleMDDataCatalog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
     <t xml:space="preserve">dcat:contactPoint</t>
   </si>
   <si>
-    <t xml:space="preserve">dcterms:license</t>
-  </si>
-  <si>
     <t xml:space="preserve">dcat:version</t>
   </si>
   <si>
-    <t xml:space="preserve">dcat:theme</t>
-  </si>
-  <si>
     <t xml:space="preserve">dcterms:spatial</t>
   </si>
   <si>
@@ -120,9 +139,6 @@
   </si>
   <si>
     <t xml:space="preserve">France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
   </si>
   <si>
     <t xml:space="preserve">12345, dsdfadf</t>
@@ -401,7 +417,7 @@
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -422,13 +438,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -480,7 +489,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -502,10 +511,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -640,9 +645,80 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.36"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -662,46 +738,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,37 +785,37 @@
         <v>12345</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>2010</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="N2" s="3" t="n">
         <v>45580</v>
@@ -750,37 +826,37 @@
         <v>73956</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>2011</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>94759</v>
@@ -791,43 +867,43 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0.4</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="N4" s="5" t="n">
         <v>45586</v>
@@ -835,40 +911,40 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>3.4</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>51</v>
+      <c r="H5" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>2019</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="N5" s="5" t="n">
         <v>45586</v>
@@ -892,14 +968,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -913,19 +989,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,13 +1009,13 @@
         <v>23456</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>45580</v>
@@ -950,13 +1026,13 @@
         <v>94759</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>45582</v>
@@ -964,36 +1040,36 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>65</v>
+      <c r="E4" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>65</v>
+        <v>72</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1013,7 +1089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1033,91 +1109,91 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1131,7 +1207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1152,87 +1228,87 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1246,7 +1322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1267,87 +1343,87 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>113</v>
+        <v>117</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>73956</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>5.46</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>115</v>
+      <c r="E2" s="7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>73956</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0.975</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>117</v>
+      <c r="E3" s="7" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>12345</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>275937582</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>119</v>
+      <c r="E4" s="7" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>121</v>
+      <c r="E5" s="7" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the rdf graph to be more EU DCAT-AP compliant
</commit_message>
<xml_diff>
--- a/tests/example_spreadsheet.xlsx
+++ b/tests/example_spreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DataCatalog" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="131">
   <si>
     <t xml:space="preserve">dcterms:title</t>
   </si>
@@ -99,66 +99,72 @@
     <t xml:space="preserve">jdoe@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">https://creativecommons.org/licenses/by/4.0/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test, catalog, energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acceptence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vgsgr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23456, 84753</t>
+  </si>
+  <si>
+    <t xml:space="preserve">derived data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a test dataset to see if we can get lineage right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jane doe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jane@example.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://opensource.org/licenses/Apache-2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lineage, catalog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12345, dsdfadf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ewrcqwfeb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existing wind on-shore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data set contains data on capacity factors of on-shore wind across different GIS regions as a time series since 1980 to 2022 on hourly basis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info@mopo.eu</t>
+  </si>
+  <si>
     <t xml:space="preserve">cc-by 4.0</t>
   </si>
   <si>
-    <t xml:space="preserve">1.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test, catalog, energy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">acceptence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23456, 84753</t>
-  </si>
-  <si>
-    <t xml:space="preserve">derived data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a test dataset to see if we can get lineage right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jane doe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jane@example.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://opensource.org/licenses/Apache-2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lineage, catalog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12345, dsdfadf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ewrcqwfeb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">existing wind on-shore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data set contains data on capacity factors of on-shore wind across different GIS regions as a time series since 1980 to 2022 on hourly basis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info@mopo.eu</t>
-  </si>
-  <si>
     <t xml:space="preserve">wind, onshore, capacity factor</t>
   </si>
   <si>
@@ -192,9 +198,6 @@
     <t xml:space="preserve">test@test.com</t>
   </si>
   <si>
-    <t xml:space="preserve">cc—by 4.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">wind, lineage</t>
   </si>
   <si>
@@ -205,6 +208,15 @@
   </si>
   <si>
     <t xml:space="preserve">asdfasdbf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">making a longer lineage chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lineage chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the prov org</t>
   </si>
   <si>
     <t xml:space="preserve">dcat:accessURL</t>
@@ -417,7 +429,7 @@
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -438,6 +450,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -489,7 +508,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -499,6 +518,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -647,56 +670,56 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="1" sqref="L2 B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -716,10 +739,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -796,7 +819,7 @@
       <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -814,10 +837,13 @@
       <c r="K2" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="N2" s="4" t="n">
         <v>45580</v>
       </c>
     </row>
@@ -825,29 +851,29 @@
       <c r="A3" s="1" t="n">
         <v>73956</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="C3" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>2011</v>
@@ -856,107 +882,122 @@
         <v>11</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>94759</v>
       </c>
-      <c r="N3" s="3" t="n">
+      <c r="N3" s="4" t="n">
         <v>45582</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0.4</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N4" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="N4" s="6" t="n">
         <v>45586</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>3.4</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>2019</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N5" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="N5" s="6" t="n">
         <v>45586</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="jdoe@example.com"/>
-    <hyperlink ref="E3" r:id="rId2" display="jane@example.org"/>
-    <hyperlink ref="F3" r:id="rId3" display="https://opensource.org/licenses/Apache-2.0"/>
-    <hyperlink ref="E4" r:id="rId4" display="info@mopo.eu"/>
-    <hyperlink ref="E5" r:id="rId5" display="test@test.com"/>
+    <hyperlink ref="F2" r:id="rId2" display="https://creativecommons.org/licenses/by/4.0/"/>
+    <hyperlink ref="E3" r:id="rId3" display="jane@example.org"/>
+    <hyperlink ref="F3" r:id="rId4" display="https://opensource.org/licenses/Apache-2.0"/>
+    <hyperlink ref="E4" r:id="rId5" display="info@mopo.eu"/>
+    <hyperlink ref="E5" r:id="rId6" display="test@test.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -976,7 +1017,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="L2 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -992,10 +1033,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1009,15 +1050,15 @@
         <v>23456</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="E2" s="4" t="n">
         <v>45580</v>
       </c>
     </row>
@@ -1026,50 +1067,50 @@
         <v>94759</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="E3" s="4" t="n">
         <v>45582</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>70</v>
+      <c r="E4" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>70</v>
+        <v>76</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1097,7 +1138,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="1" sqref="L2 E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1109,19 +1150,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,71 +1170,71 @@
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1214,8 +1255,8 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="L2 C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1231,84 +1272,84 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1346,84 +1387,84 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>118</v>
+        <v>121</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>73956</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>5.46</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>120</v>
+      <c r="E2" s="8" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="4" t="n">
+        <v>125</v>
+      </c>
+      <c r="B3" s="5" t="n">
         <v>73956</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0.975</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>122</v>
+      <c r="E3" s="8" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>12345</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>275937582</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>124</v>
+      <c r="E4" s="8" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>112</v>
+        <v>129</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>126</v>
+      <c r="E5" s="8" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>